<commit_message>
firebase & notification & Profiles
</commit_message>
<xml_diff>
--- a/palette-connection-service/src/data/SFCredentials.xlsx
+++ b/palette-connection-service/src/data/SFCredentials.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t xml:space="preserve">InstituteName</t>
   </si>
@@ -67,19 +67,34 @@
     <t xml:space="preserve">Palette123!@#</t>
   </si>
   <si>
+    <t xml:space="preserve">Palette2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3MVG9kBt168mda_8TulrtJcUfzuHJr3EkvhZ9FLFas93t7PEGX3dkQx_KxnxdqAb_480ZJNAUAz1Kbqn1Wi9o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">155CF31C83E4EDBBA594C8668316E00A5D8EF67340409F1E952BF8F5578EA90C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">palette_app@paletteedu.net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palette123@2022vFfDK0irvX7eeMJMyD1WqsqW</t>
+  </si>
+  <si>
     <t xml:space="preserve">Big Thoughts</t>
   </si>
   <si>
-    <t xml:space="preserve">3MVG9kBt168mda_8TulrtJcUfzuHJr3EkvhZ9FLFas93t7PEGX3dkQx_KxnxdqAb_480ZJNAUAz1Kbqn1Wi9o</t>
-  </si>
-  <si>
-    <t xml:space="preserve">155CF31C83E4EDBBA594C8668316E00A5D8EF67340409F1E952BF8F5578EA90C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">palette_app@paletteedu.net</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Palette123@2022vFfDK0irvX7eeMJMyD1WqsqW</t>
+    <t xml:space="preserve">3MVG9riCAn8HHkYU91QNJpiu_IyQgQ1.8HPQcAaqdCg7F0phNU4MzHGe3ul5.bls292xXryTZDmyZiiYp8Jja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EAE824E601E252A759AFC4EFAEE55C3A0ABC00C487C2E52811AE271CEF592FD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vijay@bigtpalette.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bigthought@palette1232JVdt6m4PwOEUKjY1eAl9lc7</t>
   </si>
 </sst>
 </file>
@@ -89,7 +104,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -112,14 +127,7 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <name val="Ubuntu"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <sz val="16"/>
       <name val="Ubuntu"/>
       <family val="0"/>
       <charset val="1"/>
@@ -167,24 +175,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -208,48 +208,49 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="19.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="40.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="38.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="40.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="32.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="11.59"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -275,11 +276,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+    <row r="3" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3"/>
       <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
@@ -292,22 +292,35 @@
       <c r="F3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="2"/>
+    <row r="4" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>